<commit_message>
commit of offline chat.
</commit_message>
<xml_diff>
--- a/OneDayCart/src/test/java/commonData/Search.xlsx
+++ b/OneDayCart/src/test/java/commonData/Search.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14355" windowHeight="4695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="5955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="search" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="offlinechat" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:L14"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Search products</t>
   </si>
@@ -35,12 +36,21 @@
   <si>
     <t>1 KG</t>
   </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +95,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -131,7 +149,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -163,9 +181,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -197,6 +216,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -372,16 +392,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,7 +409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -397,7 +417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -412,24 +432,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>